<commit_message>
Improved Destination and Login handling. Tax calculation for all currency types
</commit_message>
<xml_diff>
--- a/SAP_AccDoc_1-0-2_SSO.xlsx
+++ b/SAP_AccDoc_1-0-2_SSO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mh019057\source\repos\hmun\SapAccExcelAddin\SapAccExcelAddin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_WS\SapAccExcelAddin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="1212" windowWidth="12228" windowHeight="6780" tabRatio="281" activeTab="1"/>
+    <workbookView xWindow="3135" yWindow="1215" windowWidth="12225" windowHeight="6780" tabRatio="281" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,6 @@
     <definedName name="TESTVKEY">'SAP-Acc-Data'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2328,6 +2327,7 @@
     <cellStyle name="Input 2" xfId="78"/>
     <cellStyle name="Linked Cell 2" xfId="79"/>
     <cellStyle name="Neutral 2" xfId="80"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Note 2" xfId="81"/>
     <cellStyle name="Output 2" xfId="82"/>
@@ -2441,7 +2441,6 @@
     <cellStyle name="SAPReadonlyDataCell" xfId="138"/>
     <cellStyle name="SAPReadonlyDataTotalCell" xfId="141"/>
     <cellStyle name="Sheet Title" xfId="119"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="41"/>
     <cellStyle name="Total 2" xfId="120"/>
     <cellStyle name="Warning Text 2" xfId="121"/>
@@ -2753,16 +2752,16 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -2784,7 +2783,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
@@ -2832,7 +2831,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
@@ -2844,7 +2843,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>54</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>53</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>37</v>
       </c>
@@ -2898,7 +2897,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>38</v>
       </c>
@@ -2916,7 +2915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
         <v>42</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>43</v>
       </c>
@@ -2952,7 +2951,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>44</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>45</v>
       </c>
@@ -3004,58 +3003,58 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:BD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="4.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="4.109375" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="15" width="4.109375" style="14" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="18" width="4.109375" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="4.109375" style="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="23" width="4.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="4.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="4.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.140625" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="15" width="4.140625" style="14" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="18" width="4.140625" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="4.140625" style="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="23" width="4.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="4.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" style="38" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.109375" style="5" customWidth="1"/>
+    <col min="30" max="30" width="5.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.140625" style="5" customWidth="1"/>
     <col min="35" max="35" width="25" style="38" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="4.109375" style="5" customWidth="1"/>
-    <col min="38" max="38" width="4.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="4.109375" style="25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="4.109375" style="13" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="44" width="4.109375" style="45" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="4.109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4.140625" style="5" customWidth="1"/>
+    <col min="38" max="38" width="4.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="4.140625" style="25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="4.140625" style="13" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="44" width="4.140625" style="45" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="4.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.109375" style="5" customWidth="1"/>
-    <col min="54" max="54" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="69.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="20.88671875" style="40" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="11.44140625" style="5"/>
+    <col min="52" max="52" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4.140625" style="5" customWidth="1"/>
+    <col min="54" max="54" width="4.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="69.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="22" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" s="22" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="51" t="s">
         <v>62</v>
       </c>
@@ -3225,7 +3224,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>132</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>132</v>
       </c>
@@ -3301,109 +3300,109 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="59"/>
       <c r="B4" s="57"/>
       <c r="X4" s="58"/>
       <c r="AI4" s="54"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="55"/>
       <c r="B5" s="57"/>
       <c r="X5" s="58"/>
       <c r="AI5" s="54"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="59"/>
       <c r="B6" s="57"/>
       <c r="X6" s="58"/>
       <c r="AI6" s="54"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="55"/>
       <c r="B7" s="57"/>
       <c r="X7" s="58"/>
       <c r="AI7" s="54"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="55"/>
       <c r="B8" s="57"/>
       <c r="X8" s="58"/>
       <c r="AI8" s="54"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="55"/>
       <c r="B9" s="57"/>
       <c r="X9" s="58"/>
       <c r="AI9" s="54"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="B10" s="57"/>
       <c r="X10" s="58"/>
       <c r="AI10" s="54"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="55"/>
       <c r="B11" s="57"/>
       <c r="X11" s="58"/>
       <c r="AI11" s="54"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A12" s="55"/>
       <c r="B12" s="57"/>
       <c r="X12" s="58"/>
       <c r="AI12" s="54"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A13" s="55"/>
       <c r="B13" s="57"/>
       <c r="X13" s="58"/>
       <c r="AI13" s="54"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A14" s="55"/>
       <c r="B14" s="57"/>
       <c r="X14" s="58"/>
       <c r="AI14" s="54"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A15" s="55"/>
       <c r="B15" s="57"/>
       <c r="X15" s="58"/>
       <c r="AI15" s="58"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="55"/>
       <c r="B16" s="57"/>
       <c r="X16" s="58"/>
       <c r="AI16" s="54"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="55"/>
       <c r="B17" s="57"/>
       <c r="X17" s="58"/>
       <c r="AI17" s="58"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="55"/>
       <c r="B18" s="57"/>
       <c r="X18" s="58"/>
       <c r="AI18" s="54"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="55"/>
       <c r="B19" s="57"/>
       <c r="X19" s="58"/>
       <c r="AI19" s="54"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="55"/>
       <c r="B20" s="57"/>
       <c r="X20" s="58"/>
       <c r="AI20" s="54"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="55"/>
       <c r="B21" s="57"/>
       <c r="X21" s="58"/>
@@ -3428,27 +3427,27 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="61"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="62" t="s">
         <v>91</v>
       </c>
@@ -3464,8 +3463,12 @@
       <c r="F2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>"&lt;add key="""&amp;A2&amp;"0"" value="""&amp;B2&amp;""" "&amp;" /&gt;"</f>
+        <v>&lt;add key="Name0" value="MSF GTP"  /&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="64" t="s">
         <v>93</v>
       </c>
@@ -3481,8 +3484,12 @@
       <c r="F3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G10" si="0">"&lt;add key="""&amp;A3&amp;"0"" value="""&amp;B3&amp;""" "&amp;" /&gt;"</f>
+        <v>&lt;add key="Application Server0" value="172.27.6.23"  /&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>94</v>
       </c>
@@ -3498,8 +3505,12 @@
       <c r="F4">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="System Nr0" value="50"  /&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="64" t="s">
         <v>95</v>
       </c>
@@ -3515,26 +3526,42 @@
       <c r="F5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="System ID0" value="GTP"  /&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="64" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="65"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="Message Server0" value=""  /&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="64" t="s">
         <v>97</v>
       </c>
       <c r="B7" s="65"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="Logon Group0" value=""  /&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
         <v>98</v>
       </c>
       <c r="B8" s="65"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="Trace0" value=""  /&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="64" t="s">
         <v>99</v>
       </c>
@@ -3550,8 +3577,12 @@
       <c r="F9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="Client0" value="060"  /&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
         <v>92</v>
       </c>
@@ -3567,15 +3598,19 @@
       <c r="F10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;add key="Language0" value="DE"  /&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
         <v>100</v>
       </c>
       <c r="B12" s="68"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="69" t="s">
         <v>101</v>
       </c>
@@ -3583,7 +3618,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="71" t="s">
         <v>102</v>
       </c>
@@ -3591,28 +3626,40 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>128</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" ref="G15:G17" si="1">"&lt;add key="""&amp;A15&amp;"0"" value="""&amp;B15&amp;""" "&amp;" /&gt;"</f>
+        <v>&lt;add key="SncMode0" value="1"  /&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>130</v>
       </c>
       <c r="B16" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;add key="SncMyName0" value="p:CN=MH019057@MAGNA.GLOBAL"  /&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
       <c r="B17" t="s">
         <v>131</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;add key="SncPartnerName0" value="p:CN=SVC_SAP_GTP_ABAP"  /&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>